<commit_message>
add participant 240M_FM to the Alpha matlab script
</commit_message>
<xml_diff>
--- a/Analyses Scripts_R/ID_Order_for_Matlab.xlsx
+++ b/Analyses Scripts_R/ID_Order_for_Matlab.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>LK_07_04_14</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>240M_FM</t>
   </si>
 </sst>
 </file>
@@ -587,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1249,16 @@
         <v>80</v>
       </c>
     </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>